<commit_message>
Added Query Wallet Balance and P2P Transfer
</commit_message>
<xml_diff>
--- a/testdata/OnboardUserEntity.xlsx
+++ b/testdata/OnboardUserEntity.xlsx
@@ -8446,9 +8446,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -8510,24 +8510,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8556,31 +8556,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8588,36 +8564,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8632,12 +8578,66 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -8690,7 +8690,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8702,31 +8726,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8744,7 +8774,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8756,13 +8804,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8774,7 +8822,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8786,19 +8840,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8810,37 +8852,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8852,25 +8864,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8936,36 +8936,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -8990,13 +8960,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9019,6 +8993,30 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -9027,25 +9025,27 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -9054,132 +9054,132 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -9852,11 +9852,11 @@
   <dimension ref="A1:AB406"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="U322" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="Z121" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U343" sqref="U343"/>
+      <selection pane="bottomRight" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.1428571428571" defaultRowHeight="15"/>
@@ -40561,6 +40561,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AB406">
+    <extLst/>
+  </autoFilter>
   <mergeCells count="87">
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="A26:A46"/>

</xml_diff>